<commit_message>
pridavam vyslednu technicku dokumentaciu:
</commit_message>
<xml_diff>
--- a/documents/testovacie scenare/TS1-Vybavenie objednavky od zakaznika.xlsx
+++ b/documents/testovacie scenare/TS1-Vybavenie objednavky od zakaznika.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tis\PROJEKT\sklad\documents\testovacie scenare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\d\t\tis\2023\sklad\documents\testovacie scenare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F0F3A1-3A11-4B7D-9592-75C8A6590088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D15AED-E1F9-4DD3-8996-3904B1ED6E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6B9AC995-C48A-4D81-9586-0FCD7364C34C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{6B9AC995-C48A-4D81-9586-0FCD7364C34C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -34,22 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
-  <si>
-    <t>Predpoklady:</t>
-  </si>
-  <si>
-    <t>Vybavenie objednávky od zákazníka.</t>
-  </si>
-  <si>
-    <t>Názov:</t>
-  </si>
-  <si>
-    <t>Číslo kroku:</t>
-  </si>
-  <si>
-    <t>Prístup k aplikácii s právami používateľa.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Postup kroku:</t>
   </si>
@@ -405,19 +390,60 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Názov:  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vybavenie objednávky od zákazníka.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Predpoklady: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Prístup k aplikácii s právami používateľa.</t>
+    </r>
+  </si>
+  <si>
+    <t>Krok:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -445,6 +471,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -747,18 +781,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -776,10 +806,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -819,9 +849,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -847,7 +885,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2904500</xdr:colOff>
+      <xdr:colOff>2828300</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
@@ -892,7 +930,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1190,231 +1228,231 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B99CECF-26F5-4450-9331-183C90F28EAA}">
   <dimension ref="B1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="40.77734375" customWidth="1"/>
-    <col min="6" max="6" width="42.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:6" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="2:6" ht="10.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="2:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="34"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="6"/>
+      <c r="C4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="2:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="C6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="8"/>
-      <c r="C4" s="9" t="s">
+    </row>
+    <row r="7" spans="2:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="21"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="55.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="10"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="11" t="s">
+      <c r="D17" s="28"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="55.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    </row>
+    <row r="18" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>